<commit_message>
add: excel png file
</commit_message>
<xml_diff>
--- a/src/lib/task1.xlsx
+++ b/src/lib/task1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/choesun1_students_zhaw_ch/Documents/AI/Task 1/ai-task1/src/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{785FACD8-811E-3142-BF61-61DA99DA271F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1277442A-67CB-7B4F-BB2D-BAA5A4705B05}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{785FACD8-811E-3142-BF61-61DA99DA271F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D17003B8-11F9-CA4A-A301-37592388206A}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{2AF9082B-3D77-1B44-B2A0-000176AABEE6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{2AF9082B-3D77-1B44-B2A0-000176AABEE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Models</t>
   </si>
@@ -48,60 +48,10 @@
 LinearRegression</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RandomForest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Train: xxx
-Validation: xxx
-Test: xxx
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Linear Regression(xxx)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Train: xxx
-Validation: xxx
-Test: xxx</t>
-    </r>
-  </si>
-  <si>
-    <t>Dataset from week 1</t>
-  </si>
-  <si>
-    <t>- Removed outliers
-- Created new Feature m^2/room</t>
+    <t>Data_Preprocessing</t>
+  </si>
+  <si>
+    <t>Performance_Metrics</t>
   </si>
   <si>
     <r>
@@ -123,9 +73,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Train: xxx
-Validation: xxx
-Test: xxx
+      <t xml:space="preserve">Train: 311.48261790337494
+Validation: 504.01044029897446
+Test: 520.0184784783255
 </t>
     </r>
     <r>
@@ -147,10 +97,23 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Train: xxx
-Validation: xxx
-Test: xxx</t>
-    </r>
+Train: 549.392704610505
+Validation: 552.6346186045308
+Test: 565.9481423464539</t>
+    </r>
+  </si>
+  <si>
+    <t>X_train: 'rooms(number of rooms)', 'area', 'pop(population)', 'pop_dens(population density)', 'frg_pct(percentage foreigners)', 'emp(numer of employees)', 'tax_income', and 'luxurious'.
+y_train: The target variable for the training data, representing housing prices.
+X_test: A DataFrame containing the features for the testing data, which are the same as those used for training.
+Random Forest: Created new Feature m^2 / room
+Linear Regression: with Scaling pipeline
+y_test: The target variable for the testing data, representing housing prices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove missing,
+duplicates and extreme value from price
+</t>
   </si>
   <si>
     <r>
@@ -172,9 +135,9 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Train: xxx
-Validation: xxx
-Test: xxx
+Train: 290.5434340983
+Validation: 546.973478
+Test: 485.8882673920
 </t>
     </r>
     <r>
@@ -196,25 +159,10 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Train: xxx
-Validation: xxx
-Test: xxx</t>
-    </r>
-  </si>
-  <si>
-    <t>GridSearch
-Added more Data</t>
-  </si>
-  <si>
-    <t>- extract to common labels
-- Removed null values
-- Removed duplicate values</t>
-  </si>
-  <si>
-    <t>Data_Preprocessing</t>
-  </si>
-  <si>
-    <t>Performance_Metrics</t>
+Train: 550.234709097
+Validation: 558.78766559680
+Test: 518.70909876453433</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -296,6 +244,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -615,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0D1F70-40E0-5C49-858A-1C1C6B703D05}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,56 +583,40 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="356" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>